<commit_message>
[/] Changed ERD to include contract table
</commit_message>
<xml_diff>
--- a/Documentatie/ERD/Normaalvormen.xlsx
+++ b/Documentatie/ERD/Normaalvormen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Project-CCSB\Documentatie\ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257F658D-9FFD-4C4E-A001-921DFA841045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F820FB6E-86DE-4FE6-9A35-1C3DBBCE0350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F5C8919-044E-4B47-9C88-82D31DBD2896}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabel" sheetId="1" r:id="rId1"/>
     <sheet name="Normaalvormen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="54">
   <si>
     <t>Klantnummer</t>
   </si>
@@ -182,12 +178,30 @@
   </si>
   <si>
     <t>jansenbas@gmail.com</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Prijs</t>
+  </si>
+  <si>
+    <t>4m</t>
+  </si>
+  <si>
+    <t>Contractnummer</t>
+  </si>
+  <si>
+    <t>4,5m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -265,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -285,10 +299,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -607,7 +628,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +814,7 @@
       <c r="A7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -844,6 +865,9 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -852,6 +876,15 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -860,6 +893,15 @@
       <c r="B12" s="2">
         <v>35958</v>
       </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="15">
+        <v>180</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -867,6 +909,15 @@
       </c>
       <c r="B13" t="s">
         <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="15">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -880,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF64ADC-2B14-4DB4-BC01-907FA1D0B64E}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,30 +942,35 @@
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="Q1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="13"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -924,26 +980,38 @@
       <c r="E2" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="F2" s="16"/>
       <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="16"/>
+      <c r="O2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="W2" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -953,26 +1021,38 @@
       <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="W3" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -982,26 +1062,37 @@
       <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="W4" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -1011,26 +1102,38 @@
       <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="8"/>
+      <c r="O5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="S5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="U5" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="W5" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1040,26 +1143,28 @@
       <c r="E6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="I6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="U6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1069,22 +1174,24 @@
       <c r="E7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="I7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="K7" t="s">
+      <c r="K7" s="9"/>
+      <c r="M7" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="Q7" t="s">
+      <c r="S7" s="9"/>
+      <c r="U7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
@@ -1094,20 +1201,22 @@
       <c r="E8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="I8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="Q8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="U8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>45</v>
       </c>
@@ -1117,16 +1226,18 @@
       <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="I9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="M9" s="9" t="s">
+      <c r="K9" s="9"/>
+      <c r="Q9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1136,16 +1247,18 @@
       <c r="E10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="M10" s="6" t="s">
+      <c r="K10" s="9"/>
+      <c r="Q10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
@@ -1155,63 +1268,71 @@
       <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="I11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="M11" s="6" t="s">
+      <c r="K11" s="9"/>
+      <c r="Q11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="E12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="I12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="Q12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="9"/>
+      <c r="I13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="Q13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="Q14" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
@@ -1246,9 +1367,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>